<commit_message>
v010521 add router-dom +footer
</commit_message>
<xml_diff>
--- a/src/myjson/ejemploexcel.xlsx
+++ b/src/myjson/ejemploexcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\$_CoderHouse\React JS\Project VizioZoneR\VizioStore\viziostore\src\myjson\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C23E7AF-8418-48E8-BEE4-319CCA09F0D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC9CBC2-733A-4C9B-B9A5-358D0CF08D28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="690" windowWidth="28005" windowHeight="18015" activeTab="2" xr2:uid="{20F415A7-21AA-4A3F-AD72-4D8403B98674}"/>
+    <workbookView xWindow="975" yWindow="690" windowWidth="28005" windowHeight="18015" activeTab="1" xr2:uid="{20F415A7-21AA-4A3F-AD72-4D8403B98674}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="561">
   <si>
     <t>PROCESADOR</t>
   </si>
@@ -1610,13 +1610,118 @@
   </si>
   <si>
     <t>2000 a 3000</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1668,6 +1773,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1695,7 +1806,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1709,6 +1820,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2093,11 +2206,11 @@
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="4" t="e">
-        <f ca="1">_xlfn.CONCAT(J3&amp;" "&amp;K3&amp;" "&amp;L3&amp;" "&amp;M3)</f>
+        <f t="shared" ref="O3:O40" ca="1" si="0">_xlfn.CONCAT(J3&amp;" "&amp;K3&amp;" "&amp;L3&amp;" "&amp;M3)</f>
         <v>#NAME?</v>
       </c>
       <c r="P3" s="5" t="e">
-        <f ca="1">"'"&amp;O3&amp;"',"</f>
+        <f t="shared" ref="P3:P20" ca="1" si="1">"'"&amp;O3&amp;"',"</f>
         <v>#NAME?</v>
       </c>
       <c r="Q3" s="6"/>
@@ -2135,11 +2248,11 @@
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="4" t="e">
-        <f ca="1">_xlfn.CONCAT(J4&amp;" "&amp;K4&amp;" "&amp;L4&amp;" "&amp;M4)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P4" s="5" t="e">
-        <f ca="1">"'"&amp;O4&amp;"',"</f>
+        <f t="shared" ca="1" si="1"/>
         <v>#NAME?</v>
       </c>
       <c r="Q4" s="6"/>
@@ -2177,11 +2290,11 @@
       </c>
       <c r="N5" s="3"/>
       <c r="O5" s="4" t="e">
-        <f ca="1">_xlfn.CONCAT(J5&amp;" "&amp;K5&amp;" "&amp;L5&amp;" "&amp;M5)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P5" s="5" t="e">
-        <f ca="1">"'"&amp;O5&amp;"',"</f>
+        <f t="shared" ca="1" si="1"/>
         <v>#NAME?</v>
       </c>
       <c r="Q5" s="6"/>
@@ -2219,11 +2332,11 @@
       </c>
       <c r="N6" s="3"/>
       <c r="O6" s="4" t="e">
-        <f ca="1">_xlfn.CONCAT(J6&amp;" "&amp;K6&amp;" "&amp;L6&amp;" "&amp;M6)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P6" s="5" t="e">
-        <f ca="1">"'"&amp;O6&amp;"',"</f>
+        <f t="shared" ca="1" si="1"/>
         <v>#NAME?</v>
       </c>
       <c r="Q6" s="6"/>
@@ -2261,11 +2374,11 @@
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="4" t="e">
-        <f ca="1">_xlfn.CONCAT(J7&amp;" "&amp;K7&amp;" "&amp;L7&amp;" "&amp;M7)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P7" s="5" t="e">
-        <f ca="1">"'"&amp;O7&amp;"',"</f>
+        <f t="shared" ca="1" si="1"/>
         <v>#NAME?</v>
       </c>
       <c r="Q7" s="6"/>
@@ -2303,11 +2416,11 @@
       </c>
       <c r="N8" s="3"/>
       <c r="O8" s="4" t="e">
-        <f ca="1">_xlfn.CONCAT(J8&amp;" "&amp;K8&amp;" "&amp;L8&amp;" "&amp;M8)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P8" s="5" t="e">
-        <f ca="1">"'"&amp;O8&amp;"',"</f>
+        <f t="shared" ca="1" si="1"/>
         <v>#NAME?</v>
       </c>
       <c r="Q8" s="6"/>
@@ -2345,11 +2458,11 @@
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="4" t="e">
-        <f ca="1">_xlfn.CONCAT(J9&amp;" "&amp;K9&amp;" "&amp;L9&amp;" "&amp;M9)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P9" s="5" t="e">
-        <f ca="1">"'"&amp;O9&amp;"',"</f>
+        <f t="shared" ca="1" si="1"/>
         <v>#NAME?</v>
       </c>
       <c r="Q9" s="6"/>
@@ -2387,11 +2500,11 @@
       </c>
       <c r="N10" s="3"/>
       <c r="O10" s="4" t="e">
-        <f ca="1">_xlfn.CONCAT(J10&amp;" "&amp;K10&amp;" "&amp;L10&amp;" "&amp;M10)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P10" s="5" t="e">
-        <f ca="1">"'"&amp;O10&amp;"',"</f>
+        <f t="shared" ca="1" si="1"/>
         <v>#NAME?</v>
       </c>
       <c r="Q10" s="6"/>
@@ -2429,11 +2542,11 @@
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="4" t="e">
-        <f ca="1">_xlfn.CONCAT(J11&amp;" "&amp;K11&amp;" "&amp;L11&amp;" "&amp;M11)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P11" s="5" t="e">
-        <f ca="1">"'"&amp;O11&amp;"',"</f>
+        <f t="shared" ca="1" si="1"/>
         <v>#NAME?</v>
       </c>
       <c r="Q11" s="6"/>
@@ -2471,11 +2584,11 @@
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="4" t="e">
-        <f ca="1">_xlfn.CONCAT(J12&amp;" "&amp;K12&amp;" "&amp;L12&amp;" "&amp;M12)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P12" s="5" t="e">
-        <f ca="1">"'"&amp;O12&amp;"',"</f>
+        <f t="shared" ca="1" si="1"/>
         <v>#NAME?</v>
       </c>
       <c r="Q12" s="6"/>
@@ -2513,11 +2626,11 @@
       </c>
       <c r="N13" s="3"/>
       <c r="O13" s="4" t="e">
-        <f ca="1">_xlfn.CONCAT(J13&amp;" "&amp;K13&amp;" "&amp;L13&amp;" "&amp;M13)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P13" s="5" t="e">
-        <f ca="1">"'"&amp;O13&amp;"',"</f>
+        <f t="shared" ca="1" si="1"/>
         <v>#NAME?</v>
       </c>
       <c r="Q13" s="6"/>
@@ -2555,11 +2668,11 @@
       </c>
       <c r="N14" s="3"/>
       <c r="O14" s="4" t="e">
-        <f ca="1">_xlfn.CONCAT(J14&amp;" "&amp;K14&amp;" "&amp;L14&amp;" "&amp;M14)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P14" s="5" t="e">
-        <f ca="1">"'"&amp;O14&amp;"',"</f>
+        <f t="shared" ca="1" si="1"/>
         <v>#NAME?</v>
       </c>
       <c r="Q14" s="6"/>
@@ -2597,11 +2710,11 @@
       </c>
       <c r="N15" s="3"/>
       <c r="O15" s="4" t="e">
-        <f ca="1">_xlfn.CONCAT(J15&amp;" "&amp;K15&amp;" "&amp;L15&amp;" "&amp;M15)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P15" s="5" t="e">
-        <f ca="1">"'"&amp;O15&amp;"',"</f>
+        <f t="shared" ca="1" si="1"/>
         <v>#NAME?</v>
       </c>
       <c r="Q15" s="6"/>
@@ -2639,11 +2752,11 @@
       </c>
       <c r="N16" s="3"/>
       <c r="O16" s="4" t="e">
-        <f ca="1">_xlfn.CONCAT(J16&amp;" "&amp;K16&amp;" "&amp;L16&amp;" "&amp;M16)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P16" s="5" t="e">
-        <f ca="1">"'"&amp;O16&amp;"',"</f>
+        <f t="shared" ca="1" si="1"/>
         <v>#NAME?</v>
       </c>
       <c r="Q16" s="6"/>
@@ -2681,11 +2794,11 @@
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="4" t="e">
-        <f ca="1">_xlfn.CONCAT(J17&amp;" "&amp;K17&amp;" "&amp;L17&amp;" "&amp;M17)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P17" s="5" t="e">
-        <f ca="1">"'"&amp;O17&amp;"',"</f>
+        <f t="shared" ca="1" si="1"/>
         <v>#NAME?</v>
       </c>
       <c r="Q17" s="6"/>
@@ -2723,11 +2836,11 @@
       </c>
       <c r="N18" s="3"/>
       <c r="O18" s="4" t="e">
-        <f ca="1">_xlfn.CONCAT(J18&amp;" "&amp;K18&amp;" "&amp;L18&amp;" "&amp;M18)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P18" s="5" t="e">
-        <f ca="1">"'"&amp;O18&amp;"',"</f>
+        <f t="shared" ca="1" si="1"/>
         <v>#NAME?</v>
       </c>
       <c r="Q18" s="6"/>
@@ -2765,11 +2878,11 @@
       </c>
       <c r="N19" s="3"/>
       <c r="O19" s="4" t="e">
-        <f ca="1">_xlfn.CONCAT(J19&amp;" "&amp;K19&amp;" "&amp;L19&amp;" "&amp;M19)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P19" s="5" t="e">
-        <f ca="1">"'"&amp;O19&amp;"',"</f>
+        <f t="shared" ca="1" si="1"/>
         <v>#NAME?</v>
       </c>
       <c r="Q19" s="6"/>
@@ -2807,11 +2920,11 @@
       </c>
       <c r="N20" s="3"/>
       <c r="O20" s="4" t="e">
-        <f ca="1">_xlfn.CONCAT(J20&amp;" "&amp;K20&amp;" "&amp;L20&amp;" "&amp;M20)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P20" s="5" t="e">
-        <f ca="1">"'"&amp;O20&amp;"',"</f>
+        <f t="shared" ca="1" si="1"/>
         <v>#NAME?</v>
       </c>
       <c r="Q20" s="6"/>
@@ -2849,7 +2962,7 @@
       </c>
       <c r="N21" s="3"/>
       <c r="O21" s="4" t="e">
-        <f ca="1">_xlfn.CONCAT(J21&amp;" "&amp;K21&amp;" "&amp;L21&amp;" "&amp;M21)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P21" s="5"/>
@@ -2888,7 +3001,7 @@
       </c>
       <c r="N22" s="3"/>
       <c r="O22" s="4" t="e">
-        <f ca="1">_xlfn.CONCAT(J22&amp;" "&amp;K22&amp;" "&amp;L22&amp;" "&amp;M22)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P22" s="5"/>
@@ -2927,7 +3040,7 @@
       </c>
       <c r="N23" s="3"/>
       <c r="O23" s="3" t="e">
-        <f ca="1">_xlfn.CONCAT(J23&amp;" "&amp;K23&amp;" "&amp;L23&amp;" "&amp;M23)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P23" s="5"/>
@@ -2966,7 +3079,7 @@
       </c>
       <c r="N24" s="3"/>
       <c r="O24" s="3" t="e">
-        <f ca="1">_xlfn.CONCAT(J24&amp;" "&amp;K24&amp;" "&amp;L24&amp;" "&amp;M24)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P24" s="5"/>
@@ -3005,7 +3118,7 @@
       </c>
       <c r="N25" s="3"/>
       <c r="O25" s="3" t="e">
-        <f ca="1">_xlfn.CONCAT(J25&amp;" "&amp;K25&amp;" "&amp;L25&amp;" "&amp;M25)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P25" s="5"/>
@@ -3044,7 +3157,7 @@
       </c>
       <c r="N26" s="3"/>
       <c r="O26" s="3" t="e">
-        <f ca="1">_xlfn.CONCAT(J26&amp;" "&amp;K26&amp;" "&amp;L26&amp;" "&amp;M26)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P26" s="5"/>
@@ -3083,7 +3196,7 @@
       </c>
       <c r="N27" s="3"/>
       <c r="O27" s="3" t="e">
-        <f ca="1">_xlfn.CONCAT(J27&amp;" "&amp;K27&amp;" "&amp;L27&amp;" "&amp;M27)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P27" s="5"/>
@@ -3122,7 +3235,7 @@
       </c>
       <c r="N28" s="3"/>
       <c r="O28" s="3" t="e">
-        <f ca="1">_xlfn.CONCAT(J28&amp;" "&amp;K28&amp;" "&amp;L28&amp;" "&amp;M28)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P28" s="5"/>
@@ -3161,7 +3274,7 @@
       </c>
       <c r="N29" s="3"/>
       <c r="O29" s="3" t="e">
-        <f ca="1">_xlfn.CONCAT(J29&amp;" "&amp;K29&amp;" "&amp;L29&amp;" "&amp;M29)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P29" s="5"/>
@@ -3200,7 +3313,7 @@
       </c>
       <c r="N30" s="3"/>
       <c r="O30" s="3" t="e">
-        <f ca="1">_xlfn.CONCAT(J30&amp;" "&amp;K30&amp;" "&amp;L30&amp;" "&amp;M30)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P30" s="5"/>
@@ -3239,7 +3352,7 @@
       </c>
       <c r="N31" s="3"/>
       <c r="O31" s="3" t="e">
-        <f ca="1">_xlfn.CONCAT(J31&amp;" "&amp;K31&amp;" "&amp;L31&amp;" "&amp;M31)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P31" s="5"/>
@@ -3278,7 +3391,7 @@
       </c>
       <c r="N32" s="3"/>
       <c r="O32" s="3" t="e">
-        <f ca="1">_xlfn.CONCAT(J32&amp;" "&amp;K32&amp;" "&amp;L32&amp;" "&amp;M32)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P32" s="5"/>
@@ -3317,7 +3430,7 @@
       </c>
       <c r="N33" s="3"/>
       <c r="O33" s="3" t="e">
-        <f ca="1">_xlfn.CONCAT(J33&amp;" "&amp;K33&amp;" "&amp;L33&amp;" "&amp;M33)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P33" s="5"/>
@@ -3356,7 +3469,7 @@
       </c>
       <c r="N34" s="3"/>
       <c r="O34" s="3" t="e">
-        <f ca="1">_xlfn.CONCAT(J34&amp;" "&amp;K34&amp;" "&amp;L34&amp;" "&amp;M34)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P34" s="5"/>
@@ -3395,7 +3508,7 @@
       </c>
       <c r="N35" s="3"/>
       <c r="O35" s="3" t="e">
-        <f ca="1">_xlfn.CONCAT(J35&amp;" "&amp;K35&amp;" "&amp;L35&amp;" "&amp;M35)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P35" s="5"/>
@@ -3434,7 +3547,7 @@
       </c>
       <c r="N36" s="3"/>
       <c r="O36" s="3" t="e">
-        <f ca="1">_xlfn.CONCAT(J36&amp;" "&amp;K36&amp;" "&amp;L36&amp;" "&amp;M36)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P36" s="5"/>
@@ -3473,7 +3586,7 @@
       </c>
       <c r="N37" s="3"/>
       <c r="O37" s="3" t="e">
-        <f ca="1">_xlfn.CONCAT(J37&amp;" "&amp;K37&amp;" "&amp;L37&amp;" "&amp;M37)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P37" s="5"/>
@@ -3512,7 +3625,7 @@
       </c>
       <c r="N38" s="3"/>
       <c r="O38" s="3" t="e">
-        <f ca="1">_xlfn.CONCAT(J38&amp;" "&amp;K38&amp;" "&amp;L38&amp;" "&amp;M38)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P38" s="5"/>
@@ -3551,7 +3664,7 @@
       </c>
       <c r="N39" s="3"/>
       <c r="O39" s="3" t="e">
-        <f ca="1">_xlfn.CONCAT(J39&amp;" "&amp;K39&amp;" "&amp;L39&amp;" "&amp;M39)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P39" s="5"/>
@@ -3590,7 +3703,7 @@
       </c>
       <c r="N40" s="3"/>
       <c r="O40" s="3" t="e">
-        <f ca="1">_xlfn.CONCAT(J40&amp;" "&amp;K40&amp;" "&amp;L40&amp;" "&amp;M40)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="P40" s="5"/>
@@ -4387,7 +4500,7 @@
         <v>5</v>
       </c>
       <c r="P80" t="str">
-        <f t="shared" ref="P80:P113" si="0">"'"&amp;D80&amp;"',"</f>
+        <f t="shared" ref="P80:P113" si="2">"'"&amp;D80&amp;"',"</f>
         <v>'MB ASROCK A520M-HDV | AM4 AMD',</v>
       </c>
     </row>
@@ -4411,7 +4524,7 @@
         <v>9</v>
       </c>
       <c r="P81" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB ASROCK B450M-HDV R4.0 | AM4 AMD',</v>
       </c>
     </row>
@@ -4435,7 +4548,7 @@
         <v>9</v>
       </c>
       <c r="P82" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MAINBOARD GIGABYTE B450M GAMING | AM4 AMD',</v>
       </c>
     </row>
@@ -4459,7 +4572,7 @@
         <v>9</v>
       </c>
       <c r="P83" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB GIGABYTE B450M-DS3H | AM4 AMD',</v>
       </c>
     </row>
@@ -4483,7 +4596,7 @@
         <v>9</v>
       </c>
       <c r="P84" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB GIGABYTE A520M-H | AM4 AMD',</v>
       </c>
     </row>
@@ -4507,7 +4620,7 @@
         <v>9</v>
       </c>
       <c r="P85" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB GIGABYTE B450M V2 DSH3 | AM4 AMD',</v>
       </c>
     </row>
@@ -4531,7 +4644,7 @@
         <v>5</v>
       </c>
       <c r="P86" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB ASROCK B450M PRO4-F | AM4 AMD',</v>
       </c>
     </row>
@@ -4555,7 +4668,7 @@
         <v>9</v>
       </c>
       <c r="P87" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB MSI B450M PRO-M2 MAX | AM4 AMD',</v>
       </c>
     </row>
@@ -4579,7 +4692,7 @@
         <v>5</v>
       </c>
       <c r="P88" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB ASROCK B550M-HDV | AM4 AMD',</v>
       </c>
     </row>
@@ -4603,7 +4716,7 @@
         <v>16</v>
       </c>
       <c r="P89" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB ASUS PRIME B450M-A | AM4 AMD',</v>
       </c>
     </row>
@@ -4627,7 +4740,7 @@
         <v>5</v>
       </c>
       <c r="P90" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB GIGABYTE B450 AORUS M | AM4 AMD',</v>
       </c>
     </row>
@@ -4651,7 +4764,7 @@
         <v>5</v>
       </c>
       <c r="P91" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB GIGABYTE B450 AORUS ELITE | AM4 AMD',</v>
       </c>
     </row>
@@ -4675,7 +4788,7 @@
         <v>16</v>
       </c>
       <c r="P92" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB ASROCK B450 STEEL LEGEND LED- RGB | AM4 AMD',</v>
       </c>
     </row>
@@ -4699,7 +4812,7 @@
         <v>5</v>
       </c>
       <c r="P93" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB GIGABYTE B550M DS3H | AM4 AMD',</v>
       </c>
     </row>
@@ -4723,7 +4836,7 @@
         <v>29</v>
       </c>
       <c r="P94" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB ASROCK B550M PRO 4 AM4 FUTURE | AM4 AMD',</v>
       </c>
     </row>
@@ -4747,7 +4860,7 @@
         <v>5</v>
       </c>
       <c r="P95" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB ASROCK B550M PRO 4 AM4 FUTURE | AM4 AMD',</v>
       </c>
     </row>
@@ -4771,7 +4884,7 @@
         <v>5</v>
       </c>
       <c r="P96" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB ASROCK B550 PHATOM GAMING 4 (DDR4 4733+OC) | AM4 AMD',</v>
       </c>
     </row>
@@ -4795,7 +4908,7 @@
         <v>9</v>
       </c>
       <c r="P97" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB ASROCK B550 PHATOM GAMING 4/AC SOCKET AM4 (WI-FI) | AM4 AMD',</v>
       </c>
     </row>
@@ -4819,7 +4932,7 @@
         <v>9</v>
       </c>
       <c r="P98" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB B550M AORUS ELITE | AM4 AMD',</v>
       </c>
     </row>
@@ -4843,7 +4956,7 @@
         <v>5</v>
       </c>
       <c r="P99" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB ASUS TUF GAMING B550M-PLUS | AM4 AMD',</v>
       </c>
     </row>
@@ -4867,7 +4980,7 @@
         <v>5</v>
       </c>
       <c r="P100" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB ASROCK B550M STEEL LEGEND AM4 AMD',</v>
       </c>
     </row>
@@ -4891,7 +5004,7 @@
         <v>5</v>
       </c>
       <c r="P101" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB ASUS TUF GAMING B550M-PLUS (WI-FI) | AM4 AMD',</v>
       </c>
     </row>
@@ -4915,7 +5028,7 @@
         <v>9</v>
       </c>
       <c r="P102" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB GIGABYTE X570 GAMING X | AM4 AMD',</v>
       </c>
     </row>
@@ -4939,7 +5052,7 @@
         <v>5</v>
       </c>
       <c r="P103" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB GIGABYTE B550 AORUS ELITE | AM4 AMD',</v>
       </c>
     </row>
@@ -4963,7 +5076,7 @@
         <v>16</v>
       </c>
       <c r="P104" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB ASUS ASUS PRIME X570-PRO | AM4 AMD',</v>
       </c>
     </row>
@@ -4987,7 +5100,7 @@
         <v>16</v>
       </c>
       <c r="P105" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB GIGABYTE B550 AORUS ELITE (with Dual M.2) | AM4 AMD',</v>
       </c>
     </row>
@@ -5011,7 +5124,7 @@
         <v>16</v>
       </c>
       <c r="P106" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB MSI MPG X570 GAMING PLUS | AM4 AMD',</v>
       </c>
     </row>
@@ -5035,7 +5148,7 @@
         <v>5</v>
       </c>
       <c r="P107" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB ASROCK B550 EXTREME4 | AM4 AMD',</v>
       </c>
     </row>
@@ -5059,7 +5172,7 @@
         <v>5</v>
       </c>
       <c r="P108" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB GIGABYTE B550 AORUS PRO | AM4 AMD',</v>
       </c>
     </row>
@@ -5083,7 +5196,7 @@
         <v>5</v>
       </c>
       <c r="P109" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB GIGABYTE X570 AORUS ELITE | AM4 AMD',</v>
       </c>
     </row>
@@ -5107,7 +5220,7 @@
         <v>16</v>
       </c>
       <c r="P110" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB ASUS TUF GAMING X570-PLUS WI-FI | AM4 AMD',</v>
       </c>
     </row>
@@ -5131,7 +5244,7 @@
         <v>9</v>
       </c>
       <c r="P111" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB ASUS ROG STRIX B550-E GAMING AMD RYZEN DDR4 AM4',</v>
       </c>
     </row>
@@ -5155,7 +5268,7 @@
         <v>5</v>
       </c>
       <c r="P112" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB ASUS ROG STRIX X570-E GAMING RGB | AM4 AMD',</v>
       </c>
     </row>
@@ -5179,7 +5292,7 @@
         <v>5</v>
       </c>
       <c r="P113" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>'MB ASUS TUF GAMING X570-PLUS AMD RYZEN DDR4 AM4',</v>
       </c>
     </row>
@@ -6228,7 +6341,7 @@
         <v>9</v>
       </c>
       <c r="Q159" t="str">
-        <f t="shared" ref="Q159:Q170" si="1">"'"&amp;E160&amp;"',"</f>
+        <f t="shared" ref="Q159:Q170" si="3">"'"&amp;E160&amp;"',"</f>
         <v>'VIEWMAX ENIGMAX RX 570 8GB',</v>
       </c>
     </row>
@@ -6255,7 +6368,7 @@
         <v>9</v>
       </c>
       <c r="Q160" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>'ASROCK PHANTOM GAMING D RADEON RX 570 4G',</v>
       </c>
     </row>
@@ -6282,7 +6395,7 @@
         <v>21</v>
       </c>
       <c r="Q161" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>'Tarjeta de video Gigabyte Radeon RX 570, 4GB, 256-bits',</v>
       </c>
     </row>
@@ -6309,7 +6422,7 @@
         <v>0</v>
       </c>
       <c r="Q162" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>'ASROCK PHANTOM GAMING D RADEON RX 570 8G',</v>
       </c>
     </row>
@@ -6336,7 +6449,7 @@
         <v>0</v>
       </c>
       <c r="Q163" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>'TARJ. VIDEO SAPPHIRE RADEON RX 570 8GB GDDR5 PULSE 256 BIT',</v>
       </c>
     </row>
@@ -6363,7 +6476,7 @@
         <v>9</v>
       </c>
       <c r="Q164" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>'TARJ. VIDEO SAPPHIRE RADEON RX 5500 XT 4GB GDDR6 PULSE | 128 BIT',</v>
       </c>
     </row>
@@ -6390,7 +6503,7 @@
         <v>9</v>
       </c>
       <c r="Q165" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>'ASROCK RADEON RX 5500 XT 8GB GDDR6 CHALLENGER D 8G OC | 128 BIT',</v>
       </c>
     </row>
@@ -6417,7 +6530,7 @@
         <v>9</v>
       </c>
       <c r="Q166" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>'T. VIDEO GIGABYTE RADEON RX 5500 XT 4GB GDDR6',</v>
       </c>
     </row>
@@ -6444,7 +6557,7 @@
         <v>2</v>
       </c>
       <c r="Q167" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>'Tarjeta de video ASUS ROG Strix AMD Radeon RX570 OC edition 8GB GDDR5 256-bit',</v>
       </c>
     </row>
@@ -6471,7 +6584,7 @@
         <v>9</v>
       </c>
       <c r="Q168" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>'GIGABYTE AMD RADEON RX 580 GAMING 8GB GDDR5',</v>
       </c>
     </row>
@@ -6498,7 +6611,7 @@
         <v>12</v>
       </c>
       <c r="Q169" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>'ASUS AMD ROG STRIX RX 5500XT GAMING 8GB GDDR6',</v>
       </c>
     </row>
@@ -6525,7 +6638,7 @@
         <v>8</v>
       </c>
       <c r="Q170" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>'TARJETA VIDEO AMD RADEON RX 5500XT 8GB ASUS ROG STRIX GAMING',</v>
       </c>
     </row>
@@ -6752,21 +6865,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33C749F-C094-4343-B00D-18012DAD60C5}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="103" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="103" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>469</v>
       </c>
@@ -6776,29 +6889,32 @@
       <c r="C1" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>COUNTIF(C2,$C$2:$C$36)</f>
         <v>1</v>
@@ -6806,30 +6922,33 @@
       <c r="B2">
         <v>1001</v>
       </c>
-      <c r="C2" t="str">
-        <f>TEXT(B2,"00000000")</f>
-        <v>00001001</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="11" t="s">
+        <v>526</v>
+      </c>
+      <c r="D2" s="12">
+        <f>B2</f>
+        <v>1001</v>
+      </c>
+      <c r="E2" t="s">
         <v>470</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>280</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>328</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>329</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>330</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A36" si="0">COUNTIF(C3,$C$2:$C$36)</f>
         <v>1</v>
@@ -6837,30 +6956,33 @@
       <c r="B3">
         <v>1002</v>
       </c>
-      <c r="C3" t="str">
-        <f t="shared" ref="C3:C36" si="1">TEXT(B3,"00000000")</f>
-        <v>00001002</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="11" t="s">
+        <v>527</v>
+      </c>
+      <c r="D3" s="12">
+        <f t="shared" ref="D3:D36" si="1">B3</f>
+        <v>1002</v>
+      </c>
+      <c r="E3" t="s">
         <v>470</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>289</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>331</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>107</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>108</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -6868,30 +6990,33 @@
       <c r="B4">
         <v>1003</v>
       </c>
-      <c r="C4" t="str">
+      <c r="C4" s="11" t="s">
+        <v>528</v>
+      </c>
+      <c r="D4" s="12">
         <f t="shared" si="1"/>
-        <v>00001003</v>
-      </c>
-      <c r="D4" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E4" t="s">
         <v>470</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>125</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>332</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>52</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>53</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -6899,30 +7024,33 @@
       <c r="B5">
         <v>1004</v>
       </c>
-      <c r="C5" t="str">
+      <c r="C5" s="11" t="s">
+        <v>529</v>
+      </c>
+      <c r="D5" s="12">
         <f t="shared" si="1"/>
-        <v>00001004</v>
-      </c>
-      <c r="D5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E5" t="s">
         <v>470</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>113</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>333</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>52</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>53</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -6930,30 +7058,33 @@
       <c r="B6">
         <v>1005</v>
       </c>
-      <c r="C6" t="str">
-        <f>TEXT(B6,"00000000")</f>
-        <v>00001005</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C6" s="11" t="s">
+        <v>530</v>
+      </c>
+      <c r="D6" s="12">
+        <f t="shared" si="1"/>
+        <v>1005</v>
+      </c>
+      <c r="E6" t="s">
         <v>470</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>113</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>337</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>338</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>339</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -6961,30 +7092,33 @@
       <c r="B7">
         <v>1006</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C7" s="11" t="s">
+        <v>531</v>
+      </c>
+      <c r="D7" s="12">
         <f t="shared" si="1"/>
-        <v>00001006</v>
-      </c>
-      <c r="D7" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E7" t="s">
         <v>470</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>289</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>340</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>341</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>342</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -6992,30 +7126,33 @@
       <c r="B8">
         <v>1007</v>
       </c>
-      <c r="C8" t="str">
+      <c r="C8" s="11" t="s">
+        <v>532</v>
+      </c>
+      <c r="D8" s="12">
         <f t="shared" si="1"/>
-        <v>00001007</v>
-      </c>
-      <c r="D8" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E8" t="s">
         <v>470</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>125</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>343</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>344</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>345</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7023,30 +7160,33 @@
       <c r="B9">
         <v>1008</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C9" s="11" t="s">
+        <v>533</v>
+      </c>
+      <c r="D9" s="12">
         <f t="shared" si="1"/>
-        <v>00001008</v>
-      </c>
-      <c r="D9" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E9" t="s">
         <v>470</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>113</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>346</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>344</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>345</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7054,30 +7194,33 @@
       <c r="B10">
         <v>1009</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C10" s="11" t="s">
+        <v>534</v>
+      </c>
+      <c r="D10" s="12">
         <f t="shared" si="1"/>
-        <v>00001009</v>
-      </c>
-      <c r="D10" t="s">
+        <v>1009</v>
+      </c>
+      <c r="E10" t="s">
         <v>470</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>113</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>347</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>344</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>345</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7085,30 +7228,33 @@
       <c r="B11">
         <v>1010</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C11" s="11" t="s">
+        <v>535</v>
+      </c>
+      <c r="D11" s="12">
         <f t="shared" si="1"/>
-        <v>00001010</v>
-      </c>
-      <c r="D11" t="s">
+        <v>1010</v>
+      </c>
+      <c r="E11" t="s">
         <v>470</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>289</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>348</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>55</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>56</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7116,30 +7262,33 @@
       <c r="B12">
         <v>1011</v>
       </c>
-      <c r="C12" t="str">
+      <c r="C12" s="11" t="s">
+        <v>536</v>
+      </c>
+      <c r="D12" s="12">
         <f t="shared" si="1"/>
-        <v>00001011</v>
-      </c>
-      <c r="D12" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E12" t="s">
         <v>470</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>113</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>353</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>354</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>355</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7147,30 +7296,33 @@
       <c r="B13">
         <v>1012</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C13" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="D13" s="12">
         <f t="shared" si="1"/>
-        <v>00001012</v>
-      </c>
-      <c r="D13" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E13" t="s">
         <v>470</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>125</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>356</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>357</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>358</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7178,30 +7330,33 @@
       <c r="B14">
         <v>1013</v>
       </c>
-      <c r="C14" t="str">
+      <c r="C14" s="11" t="s">
+        <v>538</v>
+      </c>
+      <c r="D14" s="12">
         <f t="shared" si="1"/>
-        <v>00001013</v>
-      </c>
-      <c r="D14" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E14" t="s">
         <v>470</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>109</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>359</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>360</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>361</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7209,30 +7364,33 @@
       <c r="B15">
         <v>1014</v>
       </c>
-      <c r="C15" t="str">
+      <c r="C15" s="11" t="s">
+        <v>539</v>
+      </c>
+      <c r="D15" s="12">
         <f t="shared" si="1"/>
-        <v>00001014</v>
-      </c>
-      <c r="D15" t="s">
+        <v>1014</v>
+      </c>
+      <c r="E15" t="s">
         <v>470</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>113</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>362</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>363</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>364</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7240,30 +7398,33 @@
       <c r="B16">
         <v>1015</v>
       </c>
-      <c r="C16" t="str">
+      <c r="C16" s="11" t="s">
+        <v>540</v>
+      </c>
+      <c r="D16" s="12">
         <f t="shared" si="1"/>
-        <v>00001015</v>
-      </c>
-      <c r="D16" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E16" t="s">
         <v>470</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>113</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>365</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>363</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>364</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7271,30 +7432,33 @@
       <c r="B17">
         <v>1016</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C17" s="11" t="s">
+        <v>541</v>
+      </c>
+      <c r="D17" s="12">
         <f t="shared" si="1"/>
-        <v>00001016</v>
-      </c>
-      <c r="D17" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E17" t="s">
         <v>470</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>302</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>366</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>367</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>368</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7302,30 +7466,33 @@
       <c r="B18">
         <v>1017</v>
       </c>
-      <c r="C18" t="str">
+      <c r="C18" s="11" t="s">
+        <v>542</v>
+      </c>
+      <c r="D18" s="12">
         <f t="shared" si="1"/>
-        <v>00001017</v>
-      </c>
-      <c r="D18" t="s">
-        <v>1</v>
+        <v>1017</v>
       </c>
       <c r="E18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
         <v>369</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>370</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>74</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>75</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7333,30 +7500,33 @@
       <c r="B19">
         <v>1018</v>
       </c>
-      <c r="C19" t="str">
+      <c r="C19" s="11" t="s">
+        <v>543</v>
+      </c>
+      <c r="D19" s="12">
         <f t="shared" si="1"/>
-        <v>00001018</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1</v>
+        <v>1018</v>
       </c>
       <c r="E19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
         <v>371</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>372</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>77</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>78</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7364,30 +7534,33 @@
       <c r="B20">
         <v>1019</v>
       </c>
-      <c r="C20" t="str">
+      <c r="C20" s="11" t="s">
+        <v>544</v>
+      </c>
+      <c r="D20" s="12">
         <f t="shared" si="1"/>
-        <v>00001019</v>
-      </c>
-      <c r="D20" t="s">
-        <v>1</v>
+        <v>1019</v>
       </c>
       <c r="E20" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
         <v>371</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>373</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>374</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>375</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7395,30 +7568,33 @@
       <c r="B21">
         <v>1020</v>
       </c>
-      <c r="C21" t="str">
+      <c r="C21" s="11" t="s">
+        <v>545</v>
+      </c>
+      <c r="D21" s="12">
         <f t="shared" si="1"/>
-        <v>00001020</v>
-      </c>
-      <c r="D21" t="s">
-        <v>1</v>
+        <v>1020</v>
       </c>
       <c r="E21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
         <v>117</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>376</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>81</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>82</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7426,30 +7602,33 @@
       <c r="B22">
         <v>1021</v>
       </c>
-      <c r="C22" t="str">
+      <c r="C22" s="11" t="s">
+        <v>546</v>
+      </c>
+      <c r="D22" s="12">
         <f t="shared" si="1"/>
-        <v>00001021</v>
-      </c>
-      <c r="D22" t="s">
-        <v>1</v>
+        <v>1021</v>
       </c>
       <c r="E22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
         <v>125</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>377</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>251</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>252</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7457,30 +7636,33 @@
       <c r="B23">
         <v>1022</v>
       </c>
-      <c r="C23" t="str">
+      <c r="C23" s="11" t="s">
+        <v>547</v>
+      </c>
+      <c r="D23" s="12">
         <f t="shared" si="1"/>
-        <v>00001022</v>
-      </c>
-      <c r="D23" t="s">
-        <v>1</v>
+        <v>1022</v>
       </c>
       <c r="E23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
         <v>117</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>378</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>167</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>168</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7488,30 +7670,33 @@
       <c r="B24">
         <v>1023</v>
       </c>
-      <c r="C24" t="str">
+      <c r="C24" s="11" t="s">
+        <v>548</v>
+      </c>
+      <c r="D24" s="12">
         <f t="shared" si="1"/>
-        <v>00001023</v>
-      </c>
-      <c r="D24" t="s">
-        <v>1</v>
+        <v>1023</v>
       </c>
       <c r="E24" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
         <v>369</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>379</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>84</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>85</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7519,30 +7704,33 @@
       <c r="B25">
         <v>1024</v>
       </c>
-      <c r="C25" t="str">
+      <c r="C25" s="11" t="s">
+        <v>549</v>
+      </c>
+      <c r="D25" s="12">
         <f t="shared" si="1"/>
-        <v>00001024</v>
-      </c>
-      <c r="D25" t="s">
-        <v>1</v>
+        <v>1024</v>
       </c>
       <c r="E25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
         <v>369</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>380</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>84</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>85</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7550,30 +7738,33 @@
       <c r="B26">
         <v>1025</v>
       </c>
-      <c r="C26" t="str">
+      <c r="C26" s="11" t="s">
+        <v>550</v>
+      </c>
+      <c r="D26" s="12">
         <f t="shared" si="1"/>
-        <v>00001025</v>
-      </c>
-      <c r="D26" t="s">
-        <v>1</v>
+        <v>1025</v>
       </c>
       <c r="E26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
         <v>117</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>381</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>255</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>256</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7581,30 +7772,33 @@
       <c r="B27">
         <v>1026</v>
       </c>
-      <c r="C27" t="str">
+      <c r="C27" s="11" t="s">
+        <v>551</v>
+      </c>
+      <c r="D27" s="12">
         <f t="shared" si="1"/>
-        <v>00001026</v>
-      </c>
-      <c r="D27" t="s">
-        <v>1</v>
+        <v>1026</v>
       </c>
       <c r="E27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
         <v>109</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>382</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>27</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>28</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7612,30 +7806,33 @@
       <c r="B28">
         <v>1027</v>
       </c>
-      <c r="C28" t="str">
+      <c r="C28" s="11" t="s">
+        <v>552</v>
+      </c>
+      <c r="D28" s="12">
         <f t="shared" si="1"/>
-        <v>00001027</v>
-      </c>
-      <c r="D28" t="s">
-        <v>1</v>
+        <v>1027</v>
       </c>
       <c r="E28" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
         <v>125</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>383</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>384</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>385</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7643,30 +7840,33 @@
       <c r="B29">
         <v>1028</v>
       </c>
-      <c r="C29" t="str">
+      <c r="C29" s="11" t="s">
+        <v>553</v>
+      </c>
+      <c r="D29" s="12">
         <f t="shared" si="1"/>
-        <v>00001028</v>
-      </c>
-      <c r="D29" t="s">
-        <v>1</v>
+        <v>1028</v>
       </c>
       <c r="E29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
         <v>109</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>386</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>265</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>266</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7674,30 +7874,33 @@
       <c r="B30">
         <v>1029</v>
       </c>
-      <c r="C30" t="str">
+      <c r="C30" s="11" t="s">
+        <v>554</v>
+      </c>
+      <c r="D30" s="12">
         <f t="shared" si="1"/>
-        <v>00001029</v>
-      </c>
-      <c r="D30" t="s">
-        <v>1</v>
+        <v>1029</v>
       </c>
       <c r="E30" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
         <v>125</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>387</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>388</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>389</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7705,30 +7908,33 @@
       <c r="B31">
         <v>1030</v>
       </c>
-      <c r="C31" t="str">
+      <c r="C31" s="11" t="s">
+        <v>555</v>
+      </c>
+      <c r="D31" s="12">
         <f t="shared" si="1"/>
-        <v>00001030</v>
-      </c>
-      <c r="D31" t="s">
-        <v>1</v>
+        <v>1030</v>
       </c>
       <c r="E31" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
         <v>125</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>390</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>269</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>270</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7736,30 +7942,33 @@
       <c r="B32">
         <v>1031</v>
       </c>
-      <c r="C32" t="str">
+      <c r="C32" s="11" t="s">
+        <v>556</v>
+      </c>
+      <c r="D32" s="12">
         <f t="shared" si="1"/>
-        <v>00001031</v>
-      </c>
-      <c r="D32" t="s">
-        <v>1</v>
+        <v>1031</v>
       </c>
       <c r="E32" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
         <v>113</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>391</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>34</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>35</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7767,30 +7976,33 @@
       <c r="B33">
         <v>1032</v>
       </c>
-      <c r="C33" t="str">
+      <c r="C33" s="11" t="s">
+        <v>557</v>
+      </c>
+      <c r="D33" s="12">
         <f t="shared" si="1"/>
-        <v>00001032</v>
-      </c>
-      <c r="D33" t="s">
-        <v>1</v>
+        <v>1032</v>
       </c>
       <c r="E33" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
         <v>117</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>392</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>393</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>394</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7798,30 +8010,33 @@
       <c r="B34">
         <v>1033</v>
       </c>
-      <c r="C34" t="str">
+      <c r="C34" s="11" t="s">
+        <v>558</v>
+      </c>
+      <c r="D34" s="12">
         <f t="shared" si="1"/>
-        <v>00001033</v>
-      </c>
-      <c r="D34" t="s">
-        <v>1</v>
+        <v>1033</v>
       </c>
       <c r="E34" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
         <v>125</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>395</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>396</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>397</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7829,30 +8044,33 @@
       <c r="B35">
         <v>1034</v>
       </c>
-      <c r="C35" t="str">
+      <c r="C35" s="11" t="s">
+        <v>559</v>
+      </c>
+      <c r="D35" s="12">
         <f t="shared" si="1"/>
-        <v>00001034</v>
-      </c>
-      <c r="D35" t="s">
-        <v>1</v>
+        <v>1034</v>
       </c>
       <c r="E35" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
         <v>109</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>398</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>399</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>400</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -7860,35 +8078,40 @@
       <c r="B36">
         <v>1035</v>
       </c>
-      <c r="C36" t="str">
+      <c r="C36" s="11" t="s">
+        <v>560</v>
+      </c>
+      <c r="D36" s="12">
         <f t="shared" si="1"/>
-        <v>00001035</v>
-      </c>
-      <c r="D36" t="s">
-        <v>1</v>
+        <v>1035</v>
       </c>
       <c r="E36" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
         <v>401</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>402</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>94</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>95</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="C40" s="7" t="s">
         <v>523</v>
       </c>
+      <c r="D40" s="7"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -7898,8 +8121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125E98BD-7C8E-4E63-A67F-12036DAC56FA}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7948,7 +8171,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>COUNTIF(C2,$C$2:$C$33)</f>
+        <f t="shared" ref="A2:A33" si="0">COUNTIF(C2,$C$2:$C$33)</f>
         <v>1</v>
       </c>
       <c r="B2">
@@ -7979,14 +8202,14 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>COUNTIF(C3,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B3">
         <v>2002</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C33" si="0">TEXT(B3,"00000000")</f>
+        <f t="shared" ref="C3:C33" si="1">TEXT(B3,"00000000")</f>
         <v>00002002</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -8010,14 +8233,14 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>COUNTIF(C4,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B4">
         <v>2003</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002003</v>
       </c>
       <c r="D4" s="9" t="s">
@@ -8041,14 +8264,14 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>COUNTIF(C5,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B5">
         <v>2004</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002004</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -8072,7 +8295,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>COUNTIF(C6,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B6">
@@ -8103,14 +8326,14 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>COUNTIF(C7,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B7">
         <v>2006</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002006</v>
       </c>
       <c r="D7" s="9" t="s">
@@ -8134,14 +8357,14 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>COUNTIF(C8,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B8">
         <v>2007</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002007</v>
       </c>
       <c r="D8" s="9" t="s">
@@ -8165,14 +8388,14 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>COUNTIF(C9,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B9">
         <v>2008</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002008</v>
       </c>
       <c r="D9" s="9" t="s">
@@ -8196,14 +8419,14 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>COUNTIF(C10,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B10">
         <v>2009</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002009</v>
       </c>
       <c r="D10" s="9" t="s">
@@ -8227,14 +8450,14 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>COUNTIF(C11,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B11">
         <v>2010</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002010</v>
       </c>
       <c r="D11" s="9" t="s">
@@ -8258,14 +8481,14 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>COUNTIF(C12,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B12">
         <v>2011</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002011</v>
       </c>
       <c r="D12" s="9" t="s">
@@ -8289,14 +8512,14 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>COUNTIF(C13,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B13">
         <v>2012</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002012</v>
       </c>
       <c r="D13" s="9" t="s">
@@ -8320,14 +8543,14 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>COUNTIF(C14,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B14">
         <v>2013</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002013</v>
       </c>
       <c r="D14" s="9" t="s">
@@ -8351,14 +8574,14 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>COUNTIF(C15,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B15">
         <v>2014</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002014</v>
       </c>
       <c r="D15" s="9" t="s">
@@ -8382,14 +8605,14 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>COUNTIF(C16,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B16">
         <v>2015</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002015</v>
       </c>
       <c r="D16" s="9" t="s">
@@ -8413,14 +8636,14 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>COUNTIF(C17,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B17">
         <v>2016</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002016</v>
       </c>
       <c r="D17" s="9" t="s">
@@ -8444,14 +8667,14 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>COUNTIF(C18,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B18">
         <v>2017</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002017</v>
       </c>
       <c r="D18" s="9" t="s">
@@ -8475,14 +8698,14 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>COUNTIF(C19,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B19">
         <v>2018</v>
       </c>
       <c r="C19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002018</v>
       </c>
       <c r="D19" s="9" t="s">
@@ -8506,14 +8729,14 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>COUNTIF(C20,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B20">
         <v>2019</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002019</v>
       </c>
       <c r="D20" s="9" t="s">
@@ -8537,14 +8760,14 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>COUNTIF(C21,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B21">
         <v>2020</v>
       </c>
       <c r="C21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002020</v>
       </c>
       <c r="D21" s="9" t="s">
@@ -8568,14 +8791,14 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>COUNTIF(C22,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B22">
         <v>2021</v>
       </c>
       <c r="C22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002021</v>
       </c>
       <c r="D22" s="9" t="s">
@@ -8599,14 +8822,14 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>COUNTIF(C23,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B23">
         <v>2022</v>
       </c>
       <c r="C23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002022</v>
       </c>
       <c r="D23" s="9" t="s">
@@ -8630,14 +8853,14 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>COUNTIF(C24,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B24">
         <v>2023</v>
       </c>
       <c r="C24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002023</v>
       </c>
       <c r="D24" s="9" t="s">
@@ -8661,14 +8884,14 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>COUNTIF(C25,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B25">
         <v>2024</v>
       </c>
       <c r="C25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002024</v>
       </c>
       <c r="D25" s="9" t="s">
@@ -8692,14 +8915,14 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>COUNTIF(C26,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B26">
         <v>2025</v>
       </c>
       <c r="C26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002025</v>
       </c>
       <c r="D26" s="9" t="s">
@@ -8723,14 +8946,14 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>COUNTIF(C27,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B27">
         <v>2026</v>
       </c>
       <c r="C27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002026</v>
       </c>
       <c r="D27" s="9" t="s">
@@ -8754,14 +8977,14 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f>COUNTIF(C28,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B28">
         <v>2027</v>
       </c>
       <c r="C28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002027</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -8785,14 +9008,14 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f>COUNTIF(C29,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B29">
         <v>2028</v>
       </c>
       <c r="C29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002028</v>
       </c>
       <c r="D29" s="9" t="s">
@@ -8816,14 +9039,14 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f>COUNTIF(C30,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B30">
         <v>2029</v>
       </c>
       <c r="C30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002029</v>
       </c>
       <c r="D30" s="9" t="s">
@@ -8847,14 +9070,14 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f>COUNTIF(C31,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B31">
         <v>2030</v>
       </c>
       <c r="C31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002030</v>
       </c>
       <c r="D31" s="9" t="s">
@@ -8878,14 +9101,14 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f>COUNTIF(C32,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B32">
         <v>2031</v>
       </c>
       <c r="C32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002031</v>
       </c>
       <c r="D32" s="9" t="s">
@@ -8909,14 +9132,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f>COUNTIF(C33,$C$2:$C$33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B33">
         <v>2032</v>
       </c>
       <c r="C33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00002032</v>
       </c>
       <c r="D33" s="9" t="s">

</xml_diff>

<commit_message>
v060621 add img v5
</commit_message>
<xml_diff>
--- a/src/myjson/ejemploexcel.xlsx
+++ b/src/myjson/ejemploexcel.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\$_CoderHouse\React JS\Project VizioZoneR\VizioStore\viziostore\src\myjson\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06092E4-11CC-4B5D-8F6D-6053946D14EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F3CE61-A23B-48AB-8817-836372DFE64E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="1500" windowWidth="28815" windowHeight="15435" activeTab="3" xr2:uid="{20F415A7-21AA-4A3F-AD72-4D8403B98674}"/>
+    <workbookView xWindow="2445" yWindow="1500" windowWidth="30825" windowHeight="15435" activeTab="4" xr2:uid="{20F415A7-21AA-4A3F-AD72-4D8403B98674}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="bdjson1" sheetId="4" r:id="rId2"/>
     <sheet name="bdjson2" sheetId="5" r:id="rId3"/>
     <sheet name="bdjson3" sheetId="6" r:id="rId4"/>
-    <sheet name="GPU" sheetId="2" r:id="rId5"/>
-    <sheet name="ram" sheetId="3" r:id="rId6"/>
+    <sheet name="bdjson4" sheetId="7" r:id="rId5"/>
+    <sheet name="GPU" sheetId="2" r:id="rId6"/>
+    <sheet name="ram" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">bdjson1!$B$78:$K$108</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$115:$H$176</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">ram!$A$1:$I$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">ram!$A$1:$I$33</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3237" uniqueCount="703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3434" uniqueCount="733">
   <si>
     <t>PROCESADOR</t>
   </si>
@@ -2145,6 +2146,96 @@
   </si>
   <si>
     <t>MOBO</t>
+  </si>
+  <si>
+    <t>https://cyccomputer.pe/34731-large_default/asus-geforce-rtx-3070-8gb-gddr6-256bits-ko-oc-pnko-rtx3070-o8g-gaming.jpg</t>
+  </si>
+  <si>
+    <t>https://asset.msi.com/resize/image/global/product/product_1606829537a7c1043ecae4c427658234e19dcdf1e5.png62405b38c58fe0f07fcef2367d8a9ba1/1024.png</t>
+  </si>
+  <si>
+    <t>https://www.sercoplus.com/18606-large_default/vga-msi-nvidia-rtx-3070-gaming-x-trio-8g.jpg</t>
+  </si>
+  <si>
+    <t>https://www.asus.com/media/global/products/fkr8blxdwrptdxeu/P_setting_xxx_0_90_end_500.png</t>
+  </si>
+  <si>
+    <t>https://cyccomputer.pe/32599-large_default/asrock-radeon-rx-5600-xt-6gb-gddr6-192-bits-challenger-oc-pn90-ga1xzz-00uanf.jpg</t>
+  </si>
+  <si>
+    <t>https://http2.mlstatic.com/D_NQ_NP_2X_826644-MPE44174979714_112020-F.webp</t>
+  </si>
+  <si>
+    <t>https://www.profesionalreview.com/wp-content/uploads/2020/01/o202001061617580463.png</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/51AqFnChOjL._SX500_SY500_CR,0,0,500,500_.jpg</t>
+  </si>
+  <si>
+    <t>https://xercom.com.pe/wp-content/uploads/2020/12/HX432C16FB3A8.jpg</t>
+  </si>
+  <si>
+    <t>https://ovalo24.com.pe/wp-content/uploads/2020/09/3778.jpg</t>
+  </si>
+  <si>
+    <t>https://http2.mlstatic.com/D_NQ_NP_2X_776063-MPE43202523810_082020-F.webp</t>
+  </si>
+  <si>
+    <t>https://media.kingston.com/kingston/product/hx-product-memory-predator-rgb-ddr4-hx429c15pb3a8-1-zm-lg.jpg</t>
+  </si>
+  <si>
+    <t>https://cyccomputer.pe/31314-large_default/memoria-16gb-ddr4-hyperx-fury-black-bus-3200mhz-pnhx432c16fb416.jpg</t>
+  </si>
+  <si>
+    <t>https://www.sercoplus.com/15881-medium_default/mem-ram-team-group-t-force-xtreem-argb.jpg</t>
+  </si>
+  <si>
+    <t>https://www.infotec.com.pe/47506-large_default/procesador-amd-ryzen-5-5600x-100100000065box-37ghz-am4.jpg</t>
+  </si>
+  <si>
+    <t>https://www.sercoplus.com/13028-large_default/procesador-amd-ryzen-7-3700x.jpg</t>
+  </si>
+  <si>
+    <t>https://cyccomputer.pe/30152-large_default/procesador-amd-ryzen-9-5900x-37ghz-70mb-12core-am4-pn100-100000061wof.jpg</t>
+  </si>
+  <si>
+    <t>https://ae01.alicdn.com/kf/H1b4c778378ba441d814ea9132a41e1fbH/Intel-Core-i3-9100F-SRF7W-BO-de-la-computadora-de-la-PC-de-escritorio-procesador-LGA1151.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.shopify.com/s/files/1/0474/7051/0229/products/i9-10900K_11a6c5c1-7f60-4158-87b3-f44fa5aa5562.jpg</t>
+  </si>
+  <si>
+    <t>https://media.ldlc.com/r1600/ld/products/00/05/66/86/LD0005668608_2.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71JTXPsKGDL._AC_SY450_.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/61J1l6bnUEL._AC_SL1000_.jpg</t>
+  </si>
+  <si>
+    <t>https://media.ldlc.com/r1600/ld/products/00/05/04/27/LD0005042731_2.jpg</t>
+  </si>
+  <si>
+    <t>https://ae01.alicdn.com/kf/H9e03071790184b12bf52fb9a6d1757c16.jpg_640x640Q90.jpg_.webp</t>
+  </si>
+  <si>
+    <t>MB ASUS PRIME X570-PRO | AM4 AMD</t>
+  </si>
+  <si>
+    <t>https://cyccomputer.pe/32568-large_default/mb-asus-prime-x570-pro-amd-ryzen-ddr4-am4-pcie-40-rgb-pn90mb11b0-m0aay0.jpg</t>
+  </si>
+  <si>
+    <t>https://http2.mlstatic.com/D_NQ_NP_856171-MPE42978379176_082020-O.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/81Dn81WtyvL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/919hzfGXZeL._AC_SL1500_.jpg</t>
+  </si>
+  <si>
+    <t>urlFuente</t>
   </si>
 </sst>
 </file>
@@ -13632,8 +13723,8 @@
   </sheetPr>
   <dimension ref="B1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15365,6 +15456,851 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E324C1F6-BE8E-4944-AB7B-15769A0318BB}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="B1:J30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" style="16" customWidth="1"/>
+    <col min="2" max="4" width="13.85546875" style="17" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="86.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="17" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="17" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="43" t="s">
+        <v>521</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>473</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>524</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>519</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>475</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>478</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>477</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>476</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="45">
+        <v>1002</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>561</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>564</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>332</v>
+      </c>
+      <c r="G3" s="28">
+        <v>5</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>567</v>
+      </c>
+      <c r="I3" s="31" t="s">
+        <v>568</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="45">
+        <v>1004</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>561</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>564</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>337</v>
+      </c>
+      <c r="G4" s="28">
+        <v>10</v>
+      </c>
+      <c r="H4" s="30" t="s">
+        <v>569</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>570</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="45">
+        <v>1006</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>561</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>564</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>346</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>571</v>
+      </c>
+      <c r="I5" s="31" t="s">
+        <v>572</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="45">
+        <v>1021</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>561</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>391</v>
+      </c>
+      <c r="G6" s="28">
+        <v>9</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>597</v>
+      </c>
+      <c r="I6" s="31" t="s">
+        <v>598</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="45">
+        <v>1022</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>561</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>392</v>
+      </c>
+      <c r="G7" s="28">
+        <v>13</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>599</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>600</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="45">
+        <v>1023</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>561</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>395</v>
+      </c>
+      <c r="G8" s="28">
+        <v>6</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>601</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>602</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="46">
+        <v>1024</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>561</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>401</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>402</v>
+      </c>
+      <c r="G9" s="32">
+        <v>3</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>603</v>
+      </c>
+      <c r="I9" s="35" t="s">
+        <v>604</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="45">
+        <v>2008</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>471</v>
+      </c>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28" t="s">
+        <v>403</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>431</v>
+      </c>
+      <c r="G10" s="28">
+        <v>9</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>615</v>
+      </c>
+      <c r="I10" s="37" t="s">
+        <v>616</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="45">
+        <v>2010</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>471</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28" t="s">
+        <v>415</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>434</v>
+      </c>
+      <c r="G11" s="28">
+        <v>5</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>617</v>
+      </c>
+      <c r="I11" s="37" t="s">
+        <v>618</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="45">
+        <v>2012</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>471</v>
+      </c>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28" t="s">
+        <v>420</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>440</v>
+      </c>
+      <c r="G12" s="28">
+        <v>3</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>619</v>
+      </c>
+      <c r="I12" s="37" t="s">
+        <v>620</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="45">
+        <v>2016</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>471</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28" t="s">
+        <v>445</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>446</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>623</v>
+      </c>
+      <c r="I13" s="37" t="s">
+        <v>624</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="45">
+        <v>2021</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>471</v>
+      </c>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28" t="s">
+        <v>415</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>459</v>
+      </c>
+      <c r="G14" s="28">
+        <v>3</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>633</v>
+      </c>
+      <c r="I14" s="37" t="s">
+        <v>634</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B15" s="45">
+        <v>2023</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>471</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28" t="s">
+        <v>407</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>463</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>627</v>
+      </c>
+      <c r="I15" s="37" t="s">
+        <v>628</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="46">
+        <v>2024</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>471</v>
+      </c>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32" t="s">
+        <v>403</v>
+      </c>
+      <c r="F16" s="33" t="s">
+        <v>464</v>
+      </c>
+      <c r="G16" s="32">
+        <v>7</v>
+      </c>
+      <c r="H16" s="32" t="s">
+        <v>637</v>
+      </c>
+      <c r="I16" s="38" t="s">
+        <v>638</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="45">
+        <v>3005</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>701</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="28">
+        <v>8</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>597</v>
+      </c>
+      <c r="I17" s="37" t="s">
+        <v>598</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="45">
+        <v>3006</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>701</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="28"/>
+      <c r="F18" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="28">
+        <v>9</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>645</v>
+      </c>
+      <c r="I18" s="37" t="s">
+        <v>646</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="45">
+        <v>3008</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>701</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="28"/>
+      <c r="F19" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>567</v>
+      </c>
+      <c r="I19" s="37" t="s">
+        <v>568</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="45">
+        <v>3011</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>701</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="28"/>
+      <c r="F20" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="28">
+        <v>1</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>653</v>
+      </c>
+      <c r="I20" s="37" t="s">
+        <v>654</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B21" s="45">
+        <v>3019</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>701</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="28"/>
+      <c r="F21" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="G21" s="28">
+        <v>10</v>
+      </c>
+      <c r="H21" s="28" t="s">
+        <v>663</v>
+      </c>
+      <c r="I21" s="37" t="s">
+        <v>664</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="46">
+        <v>3020</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>701</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="32"/>
+      <c r="F22" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="G22" s="32">
+        <v>15</v>
+      </c>
+      <c r="H22" s="32" t="s">
+        <v>565</v>
+      </c>
+      <c r="I22" s="38" t="s">
+        <v>566</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B23" s="45">
+        <v>4012</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>702</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="G23" s="29">
+        <v>9</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>679</v>
+      </c>
+      <c r="I23" s="37" t="s">
+        <v>680</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B24" s="45">
+        <v>4013</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>702</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="F24" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="G24" s="29">
+        <v>4</v>
+      </c>
+      <c r="H24" s="28" t="s">
+        <v>681</v>
+      </c>
+      <c r="I24" s="37" t="s">
+        <v>682</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B25" s="45">
+        <v>4014</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>702</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="G25" s="29">
+        <v>9</v>
+      </c>
+      <c r="H25" s="28" t="s">
+        <v>683</v>
+      </c>
+      <c r="I25" s="37" t="s">
+        <v>684</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B26" s="45">
+        <v>4015</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>702</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="F26" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="G26" s="29">
+        <v>10</v>
+      </c>
+      <c r="H26" s="28" t="s">
+        <v>685</v>
+      </c>
+      <c r="I26" s="37" t="s">
+        <v>686</v>
+      </c>
+      <c r="J26" s="16" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B27" s="45">
+        <v>4026</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>702</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" s="29" t="s">
+        <v>727</v>
+      </c>
+      <c r="G27" s="29">
+        <v>12</v>
+      </c>
+      <c r="H27" s="28" t="s">
+        <v>585</v>
+      </c>
+      <c r="I27" s="37" t="s">
+        <v>586</v>
+      </c>
+      <c r="J27" s="16" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B28" s="45">
+        <v>4028</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>702</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="G28" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>591</v>
+      </c>
+      <c r="I28" s="37" t="s">
+        <v>592</v>
+      </c>
+      <c r="J28" s="16" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B29" s="45">
+        <v>4029</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>702</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="G29" s="29">
+        <v>5</v>
+      </c>
+      <c r="H29" s="28" t="s">
+        <v>595</v>
+      </c>
+      <c r="I29" s="37" t="s">
+        <v>596</v>
+      </c>
+      <c r="J29" s="16" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="46">
+        <v>4030</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>702</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="F30" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="G30" s="33">
+        <v>8</v>
+      </c>
+      <c r="H30" s="32" t="s">
+        <v>699</v>
+      </c>
+      <c r="I30" s="38" t="s">
+        <v>700</v>
+      </c>
+      <c r="J30" s="16" t="s">
+        <v>731</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33C749F-C094-4343-B00D-18012DAD60C5}">
   <dimension ref="A1:K36"/>
   <sheetViews>
@@ -16222,7 +17158,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125E98BD-7C8E-4E63-A67F-12036DAC56FA}">
   <dimension ref="A1:L37"/>
   <sheetViews>

</xml_diff>